<commit_message>
docs: 📝 update diary
</commit_message>
<xml_diff>
--- a/journal_de_travail.xlsx
+++ b/journal_de_travail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C367BEB3-E56F-4D3B-9D76-D1776801E834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8877E51C-A6B6-4803-B096-D14F28C71E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5505" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.6597222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>4.4784722222222229</v>
+        <v>4.9506944444444452</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -918,15 +918,39 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45514</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28472222222222215</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>45520</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.75</v>
+      </c>
       <c r="D28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1875</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs: 📝 updated diary
</commit_message>
<xml_diff>
--- a/journal_de_travail.xlsx
+++ b/journal_de_travail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TB2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8877E51C-A6B6-4803-B096-D14F28C71E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8740E39-CEE2-4FA8-B856-9B6F8ECF476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -394,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>0.46527777777777779</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
       </c>
       <c r="I7" s="3">
         <f>SUM(I1:I5)</f>
-        <v>4.9506944444444452</v>
+        <v>5.2284722222222229</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -954,9 +954,21 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>45521</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.65277777777777779</v>
+      </c>
       <c r="D29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>